<commit_message>
Changes of RTE job process
</commit_message>
<xml_diff>
--- a/NetAgent/src/main/resources/NA OCP Result_PreProd.xlsx
+++ b/NetAgent/src/main/resources/NA OCP Result_PreProd.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="50">
   <si>
     <t>Service</t>
   </si>
@@ -113,45 +113,6 @@
     <t>FAIL</t>
   </si>
   <si>
-    <t>10059598</t>
-  </si>
-  <si>
-    <t>10059600</t>
-  </si>
-  <si>
-    <t>10059603</t>
-  </si>
-  <si>
-    <t>10059610</t>
-  </si>
-  <si>
-    <t>10059622</t>
-  </si>
-  <si>
-    <t>10059630</t>
-  </si>
-  <si>
-    <t>10059858</t>
-  </si>
-  <si>
-    <t>10059863</t>
-  </si>
-  <si>
-    <t>10059864</t>
-  </si>
-  <si>
-    <t>10059887</t>
-  </si>
-  <si>
-    <t>10059897</t>
-  </si>
-  <si>
-    <t>794641595264</t>
-  </si>
-  <si>
-    <t>10059903</t>
-  </si>
-  <si>
     <t>NA Process Result</t>
   </si>
   <si>
@@ -159,6 +120,60 @@
   </si>
   <si>
     <t>NA Fail Log</t>
+  </si>
+  <si>
+    <t>10146166</t>
+  </si>
+  <si>
+    <t>10165094</t>
+  </si>
+  <si>
+    <t>10165106</t>
+  </si>
+  <si>
+    <t>10165179</t>
+  </si>
+  <si>
+    <t>10165231</t>
+  </si>
+  <si>
+    <t>10165275</t>
+  </si>
+  <si>
+    <t>10165292</t>
+  </si>
+  <si>
+    <t>10165324</t>
+  </si>
+  <si>
+    <t>10165370</t>
+  </si>
+  <si>
+    <t>10165451</t>
+  </si>
+  <si>
+    <t>794643740667</t>
+  </si>
+  <si>
+    <t>10165558</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>10167505</t>
+  </si>
+  <si>
+    <t>10167521</t>
+  </si>
+  <si>
+    <t>RTE</t>
+  </si>
+  <si>
+    <t>Get TrackingNo</t>
+  </si>
+  <si>
+    <t>Process</t>
   </si>
 </sst>
 </file>
@@ -235,13 +250,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -545,7 +560,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
@@ -558,9 +573,9 @@
     <col min="3" max="3" width="19.5703125" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="17.85546875" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="23.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="40.140625" style="7" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="22.5703125" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" customWidth="1"/>
+    <col min="6" max="6" width="40.140625" style="5" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="22.5703125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -577,16 +592,16 @@
         <v>5</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -595,13 +610,15 @@
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="3" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="5"/>
+      <c r="F2" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
     </row>
@@ -611,13 +628,15 @@
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="3" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" s="5"/>
+        <v>28</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
     </row>
@@ -627,13 +646,15 @@
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" s="6"/>
+        <v>28</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
     </row>
@@ -643,13 +664,15 @@
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" s="5"/>
+        <v>28</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
     </row>
@@ -659,13 +682,15 @@
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" s="5"/>
+        <v>28</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
     </row>
@@ -675,13 +700,15 @@
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" s="5"/>
+        <v>28</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
     </row>
@@ -690,12 +717,16 @@
         <v>9</v>
       </c>
       <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
+      <c r="C8" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="D8" s="1"/>
       <c r="E8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="6"/>
+      <c r="F8" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
     </row>
@@ -705,13 +736,15 @@
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9" s="5"/>
+        <v>28</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
     </row>
@@ -721,13 +754,15 @@
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10" s="5"/>
+        <v>28</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
     </row>
@@ -737,13 +772,15 @@
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="6"/>
+      <c r="F11" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
     </row>
@@ -753,13 +790,15 @@
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F12" s="6"/>
+        <v>28</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
     </row>
@@ -769,13 +808,15 @@
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F13" s="5"/>
+        <v>28</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
     </row>
@@ -785,18 +826,22 @@
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F14" s="5"/>
+        <v>28</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
+      <c r="A15" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="B15" s="1" t="s">
         <v>6</v>
       </c>
@@ -805,12 +850,16 @@
       <c r="E15" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F15" s="5"/>
+      <c r="F15" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
+      <c r="A16" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="B16" s="1" t="s">
         <v>7</v>
       </c>
@@ -819,12 +868,16 @@
       <c r="E16" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F16" s="5"/>
+      <c r="F16" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
+      <c r="A17" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="B17" s="1" t="s">
         <v>24</v>
       </c>
@@ -833,12 +886,16 @@
       <c r="E17" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F17" s="5"/>
+      <c r="F17" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
+      <c r="A18" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="B18" s="1" t="s">
         <v>19</v>
       </c>
@@ -847,64 +904,84 @@
       <c r="E18" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F18" s="5"/>
+      <c r="F18" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
+      <c r="A19" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="B19" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
-      <c r="F19" s="5"/>
+      <c r="F19" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
+      <c r="A20" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="B20" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F20" s="5"/>
+      <c r="F20" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
+      <c r="A21" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="B21" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="5"/>
+      <c r="F21" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
+      <c r="A22" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="B22" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
-      <c r="F22" s="5"/>
+      <c r="F22" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
+      <c r="A23" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="B23" s="1" t="s">
         <v>23</v>
       </c>
@@ -913,9 +990,49 @@
       <c r="E23" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F23" s="6"/>
+      <c r="F23" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="3"/>
+      <c r="B25" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="3"/>
+      <c r="B26" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576">

</xml_diff>